<commit_message>
slight dataframe adaption and added the %notebook to better check the new graph
</commit_message>
<xml_diff>
--- a/Data_files/Part_2/Rotterdam_car_adjacency_v2.xlsx
+++ b/Data_files/Part_2/Rotterdam_car_adjacency_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimEW\PycharmProjects\Design_in_Network_group_8\Data_files\Part_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B02789F-8462-4176-A184-4922DA400840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{736F54ED-5B3E-4BE0-A3D4-197CD1A72AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -570,8 +570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="81" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="T27" sqref="T27"/>
+    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -989,10 +989,10 @@
         <v>9</v>
       </c>
       <c r="B6" s="7">
-        <v>51.952199999999998</v>
+        <v>51.918433289217802</v>
       </c>
       <c r="C6" s="7">
-        <v>4.5518999999999998</v>
+        <v>4.4739989821962398</v>
       </c>
       <c r="D6" s="7">
         <v>41190</v>
@@ -2333,6 +2333,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000967D3B9FC1DD84EB00B55E5790AB85E" ma:contentTypeVersion="4" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="92ec66a21d0d7142cf1fb1ae8fa08641">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6ba023f1-a19b-4eec-904c-052d1f1cb5e0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="62a86672aac255264bf3f3decc56659c" ns2:_="">
     <xsd:import namespace="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
@@ -2476,35 +2491,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47226C14-663C-468E-81A1-C92460C7FBF2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4089522E-0C82-47E8-A49E-84CDA0FE73C2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2526,9 +2516,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4089522E-0C82-47E8-A49E-84CDA0FE73C2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47226C14-663C-468E-81A1-C92460C7FBF2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>